<commit_message>
Se agregan las solapas de calendarios, avances.
</commit_message>
<xml_diff>
--- a/Información.xlsx
+++ b/Información.xlsx
@@ -1,21 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="16275" windowHeight="4935" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="15480" windowHeight="4935" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Roles" sheetId="1" r:id="rId1"/>
     <sheet name="Herramientas" sheetId="2" r:id="rId2"/>
+    <sheet name="Calendario(interno)" sheetId="3" r:id="rId3"/>
+    <sheet name="Calendario(Cliente)" sheetId="4" r:id="rId4"/>
+    <sheet name="Avances" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="23">
   <si>
     <t>Diego Martinez</t>
   </si>
@@ -36,13 +39,75 @@
   </si>
   <si>
     <t>MySQL</t>
+  </si>
+  <si>
+    <t>Domingo</t>
+  </si>
+  <si>
+    <t>Lunes</t>
+  </si>
+  <si>
+    <t>Martes</t>
+  </si>
+  <si>
+    <t>Miercoles</t>
+  </si>
+  <si>
+    <t>Jueves</t>
+  </si>
+  <si>
+    <t>Viernes</t>
+  </si>
+  <si>
+    <t>Sabado</t>
+  </si>
+  <si>
+    <t>Mes</t>
+  </si>
+  <si>
+    <t>Agosto</t>
+  </si>
+  <si>
+    <t>Septiembre</t>
+  </si>
+  <si>
+    <t>Octubre</t>
+  </si>
+  <si>
+    <t>Nobiembre</t>
+  </si>
+  <si>
+    <t>25
+Armado ypresentación del equipo</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">8
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Presentación del equipo y de las herramientas a utilizar</t>
+    </r>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>Desarrollador</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -50,8 +115,38 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -61,6 +156,30 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -92,11 +211,41 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -112,7 +261,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -186,7 +335,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -221,7 +369,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -397,86 +544,91 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
+    <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:5">
+      <c r="A1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="10" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
+    <row r="2" spans="1:5">
+      <c r="A2" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="10"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="10"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="10"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="10"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="10"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -485,21 +637,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -507,4 +659,858 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="6" width="15.7109375" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="60">
+      <c r="A2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="1">
+        <v>23</v>
+      </c>
+      <c r="C2" s="1">
+        <v>24</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="1">
+        <v>26</v>
+      </c>
+      <c r="F2" s="1">
+        <v>27</v>
+      </c>
+      <c r="G2" s="1">
+        <v>28</v>
+      </c>
+      <c r="H2" s="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="7"/>
+      <c r="B3" s="1">
+        <v>30</v>
+      </c>
+      <c r="C3" s="1">
+        <v>31</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="1">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1">
+        <v>2</v>
+      </c>
+      <c r="F4" s="1">
+        <v>3</v>
+      </c>
+      <c r="G4" s="1">
+        <v>4</v>
+      </c>
+      <c r="H4" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="75">
+      <c r="A5" s="7"/>
+      <c r="B5" s="1">
+        <v>6</v>
+      </c>
+      <c r="C5" s="1">
+        <v>7</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="1">
+        <v>9</v>
+      </c>
+      <c r="F5" s="1">
+        <v>10</v>
+      </c>
+      <c r="G5" s="1">
+        <v>11</v>
+      </c>
+      <c r="H5" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="7"/>
+      <c r="B6" s="1">
+        <v>13</v>
+      </c>
+      <c r="C6" s="1">
+        <v>14</v>
+      </c>
+      <c r="D6" s="1">
+        <v>15</v>
+      </c>
+      <c r="E6" s="1">
+        <v>16</v>
+      </c>
+      <c r="F6" s="1">
+        <v>17</v>
+      </c>
+      <c r="G6" s="1">
+        <v>18</v>
+      </c>
+      <c r="H6" s="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="7"/>
+      <c r="B7" s="1">
+        <v>20</v>
+      </c>
+      <c r="C7" s="1">
+        <v>21</v>
+      </c>
+      <c r="D7" s="1">
+        <v>22</v>
+      </c>
+      <c r="E7" s="1">
+        <v>23</v>
+      </c>
+      <c r="F7" s="1">
+        <v>24</v>
+      </c>
+      <c r="G7" s="1">
+        <v>25</v>
+      </c>
+      <c r="H7" s="1">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="7"/>
+      <c r="B8" s="1">
+        <v>27</v>
+      </c>
+      <c r="C8" s="1">
+        <v>28</v>
+      </c>
+      <c r="D8" s="1">
+        <v>29</v>
+      </c>
+      <c r="E8" s="1">
+        <v>30</v>
+      </c>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="1">
+        <v>1</v>
+      </c>
+      <c r="G9" s="1">
+        <v>2</v>
+      </c>
+      <c r="H9" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="7"/>
+      <c r="B10" s="1">
+        <v>4</v>
+      </c>
+      <c r="C10" s="1">
+        <v>5</v>
+      </c>
+      <c r="D10" s="1">
+        <v>6</v>
+      </c>
+      <c r="E10" s="1">
+        <v>7</v>
+      </c>
+      <c r="F10" s="1">
+        <v>8</v>
+      </c>
+      <c r="G10" s="1">
+        <v>9</v>
+      </c>
+      <c r="H10" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="7"/>
+      <c r="B11" s="1">
+        <v>11</v>
+      </c>
+      <c r="C11" s="1">
+        <v>12</v>
+      </c>
+      <c r="D11" s="1">
+        <v>13</v>
+      </c>
+      <c r="E11" s="1">
+        <v>14</v>
+      </c>
+      <c r="F11" s="1">
+        <v>15</v>
+      </c>
+      <c r="G11" s="1">
+        <v>16</v>
+      </c>
+      <c r="H11" s="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="7"/>
+      <c r="B12" s="1">
+        <v>18</v>
+      </c>
+      <c r="C12" s="1">
+        <v>19</v>
+      </c>
+      <c r="D12" s="1">
+        <v>20</v>
+      </c>
+      <c r="E12" s="1">
+        <v>21</v>
+      </c>
+      <c r="F12" s="1">
+        <v>22</v>
+      </c>
+      <c r="G12" s="1">
+        <v>23</v>
+      </c>
+      <c r="H12" s="1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="7"/>
+      <c r="B13" s="1">
+        <v>25</v>
+      </c>
+      <c r="C13" s="1">
+        <v>26</v>
+      </c>
+      <c r="D13" s="1">
+        <v>27</v>
+      </c>
+      <c r="E13" s="1">
+        <v>28</v>
+      </c>
+      <c r="F13" s="1">
+        <v>29</v>
+      </c>
+      <c r="G13" s="1">
+        <v>30</v>
+      </c>
+      <c r="H13" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="1">
+        <v>1</v>
+      </c>
+      <c r="C14" s="1">
+        <v>2</v>
+      </c>
+      <c r="D14" s="1">
+        <v>3</v>
+      </c>
+      <c r="E14" s="1">
+        <v>4</v>
+      </c>
+      <c r="F14" s="1">
+        <v>5</v>
+      </c>
+      <c r="G14" s="1">
+        <v>6</v>
+      </c>
+      <c r="H14" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="7"/>
+      <c r="B15" s="1">
+        <v>8</v>
+      </c>
+      <c r="C15" s="1">
+        <v>9</v>
+      </c>
+      <c r="D15" s="1">
+        <v>10</v>
+      </c>
+      <c r="E15" s="1">
+        <v>11</v>
+      </c>
+      <c r="F15" s="1">
+        <v>12</v>
+      </c>
+      <c r="G15" s="1">
+        <v>13</v>
+      </c>
+      <c r="H15" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="7"/>
+      <c r="B16" s="1">
+        <v>15</v>
+      </c>
+      <c r="C16" s="1">
+        <v>16</v>
+      </c>
+      <c r="D16" s="1">
+        <v>17</v>
+      </c>
+      <c r="E16" s="1">
+        <v>18</v>
+      </c>
+      <c r="F16" s="1">
+        <v>19</v>
+      </c>
+      <c r="G16" s="1">
+        <v>20</v>
+      </c>
+      <c r="H16" s="1">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="7"/>
+      <c r="B17" s="1">
+        <v>22</v>
+      </c>
+      <c r="C17" s="1">
+        <v>23</v>
+      </c>
+      <c r="D17" s="1">
+        <v>24</v>
+      </c>
+      <c r="E17" s="1">
+        <v>25</v>
+      </c>
+      <c r="F17" s="1">
+        <v>26</v>
+      </c>
+      <c r="G17" s="1">
+        <v>27</v>
+      </c>
+      <c r="H17" s="1">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="7"/>
+      <c r="B18" s="1">
+        <v>29</v>
+      </c>
+      <c r="C18" s="1">
+        <v>30</v>
+      </c>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="1">
+        <v>23</v>
+      </c>
+      <c r="C2" s="1">
+        <v>24</v>
+      </c>
+      <c r="D2" s="1">
+        <v>25</v>
+      </c>
+      <c r="E2" s="1">
+        <v>26</v>
+      </c>
+      <c r="F2" s="1">
+        <v>27</v>
+      </c>
+      <c r="G2" s="1">
+        <v>28</v>
+      </c>
+      <c r="H2" s="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="7"/>
+      <c r="B3" s="1">
+        <v>30</v>
+      </c>
+      <c r="C3" s="1">
+        <v>31</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="1">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1">
+        <v>2</v>
+      </c>
+      <c r="F4" s="1">
+        <v>3</v>
+      </c>
+      <c r="G4" s="1">
+        <v>4</v>
+      </c>
+      <c r="H4" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="7"/>
+      <c r="B5" s="1">
+        <v>6</v>
+      </c>
+      <c r="C5" s="1">
+        <v>7</v>
+      </c>
+      <c r="D5" s="1">
+        <v>8</v>
+      </c>
+      <c r="E5" s="1">
+        <v>9</v>
+      </c>
+      <c r="F5" s="1">
+        <v>10</v>
+      </c>
+      <c r="G5" s="1">
+        <v>11</v>
+      </c>
+      <c r="H5" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="7"/>
+      <c r="B6" s="1">
+        <v>13</v>
+      </c>
+      <c r="C6" s="1">
+        <v>14</v>
+      </c>
+      <c r="D6" s="1">
+        <v>15</v>
+      </c>
+      <c r="E6" s="1">
+        <v>16</v>
+      </c>
+      <c r="F6" s="1">
+        <v>17</v>
+      </c>
+      <c r="G6" s="1">
+        <v>18</v>
+      </c>
+      <c r="H6" s="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="7"/>
+      <c r="B7" s="1">
+        <v>20</v>
+      </c>
+      <c r="C7" s="1">
+        <v>21</v>
+      </c>
+      <c r="D7" s="1">
+        <v>22</v>
+      </c>
+      <c r="E7" s="1">
+        <v>23</v>
+      </c>
+      <c r="F7" s="1">
+        <v>24</v>
+      </c>
+      <c r="G7" s="1">
+        <v>25</v>
+      </c>
+      <c r="H7" s="1">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="7"/>
+      <c r="B8" s="1">
+        <v>27</v>
+      </c>
+      <c r="C8" s="1">
+        <v>28</v>
+      </c>
+      <c r="D8" s="1">
+        <v>29</v>
+      </c>
+      <c r="E8" s="1">
+        <v>30</v>
+      </c>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="1">
+        <v>1</v>
+      </c>
+      <c r="G9" s="1">
+        <v>2</v>
+      </c>
+      <c r="H9" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="7"/>
+      <c r="B10" s="1">
+        <v>4</v>
+      </c>
+      <c r="C10" s="1">
+        <v>5</v>
+      </c>
+      <c r="D10" s="1">
+        <v>6</v>
+      </c>
+      <c r="E10" s="1">
+        <v>7</v>
+      </c>
+      <c r="F10" s="1">
+        <v>8</v>
+      </c>
+      <c r="G10" s="1">
+        <v>9</v>
+      </c>
+      <c r="H10" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="7"/>
+      <c r="B11" s="1">
+        <v>11</v>
+      </c>
+      <c r="C11" s="1">
+        <v>12</v>
+      </c>
+      <c r="D11" s="1">
+        <v>13</v>
+      </c>
+      <c r="E11" s="1">
+        <v>14</v>
+      </c>
+      <c r="F11" s="1">
+        <v>15</v>
+      </c>
+      <c r="G11" s="1">
+        <v>16</v>
+      </c>
+      <c r="H11" s="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="7"/>
+      <c r="B12" s="1">
+        <v>18</v>
+      </c>
+      <c r="C12" s="1">
+        <v>19</v>
+      </c>
+      <c r="D12" s="1">
+        <v>20</v>
+      </c>
+      <c r="E12" s="1">
+        <v>21</v>
+      </c>
+      <c r="F12" s="1">
+        <v>22</v>
+      </c>
+      <c r="G12" s="1">
+        <v>23</v>
+      </c>
+      <c r="H12" s="1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="7"/>
+      <c r="B13" s="1">
+        <v>25</v>
+      </c>
+      <c r="C13" s="1">
+        <v>26</v>
+      </c>
+      <c r="D13" s="1">
+        <v>27</v>
+      </c>
+      <c r="E13" s="1">
+        <v>28</v>
+      </c>
+      <c r="F13" s="1">
+        <v>29</v>
+      </c>
+      <c r="G13" s="1">
+        <v>30</v>
+      </c>
+      <c r="H13" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="1">
+        <v>1</v>
+      </c>
+      <c r="C14" s="1">
+        <v>2</v>
+      </c>
+      <c r="D14" s="1">
+        <v>3</v>
+      </c>
+      <c r="E14" s="1">
+        <v>4</v>
+      </c>
+      <c r="F14" s="1">
+        <v>5</v>
+      </c>
+      <c r="G14" s="1">
+        <v>6</v>
+      </c>
+      <c r="H14" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="7"/>
+      <c r="B15" s="1">
+        <v>8</v>
+      </c>
+      <c r="C15" s="1">
+        <v>9</v>
+      </c>
+      <c r="D15" s="1">
+        <v>10</v>
+      </c>
+      <c r="E15" s="1">
+        <v>11</v>
+      </c>
+      <c r="F15" s="1">
+        <v>12</v>
+      </c>
+      <c r="G15" s="1">
+        <v>13</v>
+      </c>
+      <c r="H15" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="7"/>
+      <c r="B16" s="1">
+        <v>15</v>
+      </c>
+      <c r="C16" s="1">
+        <v>16</v>
+      </c>
+      <c r="D16" s="1">
+        <v>17</v>
+      </c>
+      <c r="E16" s="1">
+        <v>18</v>
+      </c>
+      <c r="F16" s="1">
+        <v>19</v>
+      </c>
+      <c r="G16" s="1">
+        <v>20</v>
+      </c>
+      <c r="H16" s="1">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="7"/>
+      <c r="B17" s="1">
+        <v>22</v>
+      </c>
+      <c r="C17" s="1">
+        <v>23</v>
+      </c>
+      <c r="D17" s="1">
+        <v>24</v>
+      </c>
+      <c r="E17" s="1">
+        <v>25</v>
+      </c>
+      <c r="F17" s="1">
+        <v>26</v>
+      </c>
+      <c r="G17" s="1">
+        <v>27</v>
+      </c>
+      <c r="H17" s="1">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="7"/>
+      <c r="B18" s="1">
+        <v>29</v>
+      </c>
+      <c r="C18" s="1">
+        <v>30</v>
+      </c>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>